<commit_message>
added spark on hbase article
</commit_message>
<xml_diff>
--- a/artifacts/project/HDInsight Dev Guide Status.xlsx
+++ b/artifacts/project/HDInsight Dev Guide Status.xlsx
@@ -1161,9 +1161,6 @@
     <t>hdinsight-hbase-backup-replication.md</t>
   </si>
   <si>
-    <t>Is there a specific approach desired and particular libraries intended for use here?</t>
-  </si>
-  <si>
     <t>hdinsight-spark-rdd-vs-dataframe-vs-dataset.md</t>
   </si>
   <si>
@@ -1177,6 +1174,9 @@
   </si>
   <si>
     <t>hdinsight-hbase-phoenix-squirrel-linux.md</t>
+  </si>
+  <si>
+    <t>hdinsight-using-spark-to-query-hbase.md</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1726,8 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1954,7 +1954,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>208</v>
@@ -1962,18 +1962,18 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="4"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H11" s="5"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="3" t="s">
-        <v>375</v>
-      </c>
+      <c r="L11" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="M11" s="3"/>
     </row>
     <row r="12" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
@@ -2066,7 +2066,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
       <c r="L18" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M18" s="3"/>
     </row>
@@ -2080,14 +2080,14 @@
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
       <c r="L19" s="12" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M19" s="3"/>
     </row>
@@ -2337,7 +2337,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="4"/>
       <c r="L35" s="12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M35" s="3"/>
     </row>
@@ -4000,8 +4000,8 @@
   <dimension ref="A1:Q128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4135,7 +4135,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
       <c r="L6" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>297</v>

</xml_diff>

<commit_message>
Updated hbase backup article to include guidance on Phoenix
</commit_message>
<xml_diff>
--- a/artifacts/project/HDInsight Dev Guide Status.xlsx
+++ b/artifacts/project/HDInsight Dev Guide Status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18820" yWindow="460" windowWidth="27600" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="51100" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone 2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="384">
   <si>
     <t>Topic</t>
   </si>
@@ -1177,6 +1177,15 @@
   </si>
   <si>
     <t>hdinsight-using-spark-to-query-hbase.md</t>
+  </si>
+  <si>
+    <t>Suggest pulling in content from https://blogs.msdn.microsoft.com/azuredatalake/2016/09/02/hdinsight-hbase-9-things-you-must-do-to-get-great-hbase-performance/</t>
+  </si>
+  <si>
+    <t>Propose we rename this file since SQLLine is coverred and squirrel is not</t>
+  </si>
+  <si>
+    <t>Backup/replication of Phoenix is covered in this article as well.</t>
   </si>
 </sst>
 </file>
@@ -1726,8 +1735,8 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2015,7 +2024,7 @@
       <c r="L13" s="12"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>211</v>
@@ -2028,9 +2037,13 @@
       <c r="H14" s="5"/>
       <c r="I14" s="4"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L14" s="12"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
@@ -2070,7 +2083,7 @@
       </c>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>214</v>
@@ -2078,7 +2091,9 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="4" t="s">
         <v>378</v>
       </c>
@@ -2089,7 +2104,9 @@
       <c r="L19" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="M19" s="3"/>
+      <c r="M19" s="3" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
@@ -2138,13 +2155,19 @@
       <c r="D22" s="3"/>
       <c r="E22" s="4"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="3"/>
+      <c r="L22" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
@@ -2176,9 +2199,13 @@
       <c r="H24" s="5"/>
       <c r="I24" s="4"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="4"/>
+      <c r="K24" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L24" s="12"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="3" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="25" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>

</xml_diff>

<commit_message>
Updated hdinsight dev status guide
</commit_message>
<xml_diff>
--- a/artifacts/project/HDInsight Dev Guide Status.xlsx
+++ b/artifacts/project/HDInsight Dev Guide Status.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="51100" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="360" yWindow="640" windowWidth="30220" windowHeight="18040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone 2" sheetId="2" r:id="rId1"/>
     <sheet name="Milestone 1" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Milestone 1'!$A$1:$M$1</definedName>
+  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="404">
   <si>
     <t>Topic</t>
   </si>
@@ -1107,24 +1110,15 @@
     <t>add adls, ad distcp, cloudxplorer, flume, change title (upload data to HDInsight), azcopy on linux, pull in content from Sqoop. Update to include ADLS as a target.</t>
   </si>
   <si>
-    <t>Duplicate of the topics in Troubleshooting chapter above?</t>
-  </si>
-  <si>
     <t>Should this guidance be a part of the hdinsight-architecture article, in the section on storage? What's the reasoning here?</t>
   </si>
   <si>
-    <t>Any particular "common errors" you already have in mind?</t>
-  </si>
-  <si>
     <t>Is there a specific custom program we should focus on?</t>
   </si>
   <si>
     <t>Synchronize On-prem Data/Metadata with Cloud</t>
   </si>
   <si>
-    <t>Do you have specific topics to cover?</t>
-  </si>
-  <si>
     <t>Advanced Settings</t>
   </si>
   <si>
@@ -1146,9 +1140,6 @@
     <t>Replication is covered in hdinsight-hbase-replication</t>
   </si>
   <si>
-    <t>See https://channel9.msdn.com/Events/Machine-Learning-and-Data-Sciences-Conference/Data-Science-Summit-2016/MSDSS25</t>
-  </si>
-  <si>
     <t>Skip as this is not yet supported.</t>
   </si>
   <si>
@@ -1186,6 +1177,81 @@
   </si>
   <si>
     <t>Backup/replication of Phoenix is covered in this article as well.</t>
+  </si>
+  <si>
+    <t>hdinsight-hbase-phoenix-performance.md</t>
+  </si>
+  <si>
+    <t>hdinsight-debug-ambari-tez-view</t>
+  </si>
+  <si>
+    <t>Already covered in hdinsight-debug-ambari-tez-view</t>
+  </si>
+  <si>
+    <t>hdinsight-phoenix-psql.md</t>
+  </si>
+  <si>
+    <t>hdinsight-using-phoenix-query-server-rest-sdk.md</t>
+  </si>
+  <si>
+    <t>H2O</t>
+  </si>
+  <si>
+    <t>Datameer</t>
+  </si>
+  <si>
+    <t>Streamsets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hdinsight-apps-install-applications.md </t>
+  </si>
+  <si>
+    <t>hdinsight-install-published-app-h2o.md</t>
+  </si>
+  <si>
+    <t>AND hdinsight-install-published-app-datameer.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hdinsight-install-published-app-streamsets.md</t>
+  </si>
+  <si>
+    <t>hdinsight-extend-hadoop-virtual-network.md</t>
+  </si>
+  <si>
+    <t>AtScale</t>
+  </si>
+  <si>
+    <t>Dataiku</t>
+  </si>
+  <si>
+    <t>Talena</t>
+  </si>
+  <si>
+    <t>Cask</t>
+  </si>
+  <si>
+    <t>blocked getting access</t>
+  </si>
+  <si>
+    <t>Already covered by https://azure.microsoft.com/en-us/blog/introducing-dataiku-s-dss-on-microsoft-azure-hdinsight-to-make-data-science-easier/</t>
+  </si>
+  <si>
+    <t>Already covered by https://blogs.msdn.microsoft.com/azuredatalake/2016/10/17/using-cask-data-application-platform-on-azure-hdinsight/</t>
+  </si>
+  <si>
+    <t>blocked waiting for Talena to post instructions in about a month</t>
+  </si>
+  <si>
+    <t>Duplicate of the topics in Troubleshooting chapter above per Bhanu.</t>
+  </si>
+  <si>
+    <t>The idea is to cover all necessary debugging and troubleshooting steps. There are some captured here https://docs.microsoft.com/en-us/azure/hdinsight/hdinsight-hadoop-linux-information but it doesn’t cover all the scenario.
+You can also refer EMR developer guide  and management guide on different aspects that are covered to ensure what else we can add.
+http://docs.aws.amazon.com/emr/latest/ManagementGuide/emr-mgmt.pdf
+http://docs.aws.amazon.com/emr/latest/DeveloperGuide/emr-dg.pdf</t>
+  </si>
+  <si>
+    <t>same as above</t>
   </si>
 </sst>
 </file>
@@ -1732,11 +1798,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M130"/>
+  <dimension ref="A1:M136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q22" sqref="Q22"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,10 +1888,10 @@
         <v>46</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -1845,10 +1911,10 @@
         <v>46</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -1867,7 +1933,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
       <c r="L6" s="12" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="M6" s="3"/>
     </row>
@@ -1911,7 +1977,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="4"/>
       <c r="L8" s="12" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="M8" s="3"/>
     </row>
@@ -1957,10 +2023,10 @@
       <c r="J10" s="5"/>
       <c r="K10" s="4"/>
       <c r="L10" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -1980,7 +2046,7 @@
       <c r="J11" s="5"/>
       <c r="K11" s="4"/>
       <c r="L11" s="12" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="M11" s="3"/>
     </row>
@@ -2002,7 +2068,7 @@
       </c>
       <c r="L12" s="12"/>
       <c r="M12" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -2016,7 +2082,9 @@
         <v>46</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H13" s="5"/>
       <c r="I13" s="4"/>
       <c r="J13" s="5"/>
@@ -2042,7 +2110,7 @@
       </c>
       <c r="L14" s="12"/>
       <c r="M14" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -2079,7 +2147,7 @@
       <c r="J18" s="5"/>
       <c r="K18" s="4"/>
       <c r="L18" s="12" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="M18" s="3"/>
     </row>
@@ -2095,17 +2163,17 @@
         <v>46</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5"/>
       <c r="K19" s="4"/>
       <c r="L19" s="12" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2119,12 +2187,16 @@
         <v>46</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H20" s="5"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="12"/>
+      <c r="L20" s="12" t="s">
+        <v>383</v>
+      </c>
       <c r="M20" s="3"/>
     </row>
     <row r="21" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2138,12 +2210,16 @@
         <v>46</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="4"/>
+      <c r="G21" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H21" s="5"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="12"/>
+      <c r="L21" s="12" t="s">
+        <v>384</v>
+      </c>
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2163,10 +2239,10 @@
       <c r="J22" s="5"/>
       <c r="K22" s="4"/>
       <c r="L22" s="12" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2204,7 +2280,7 @@
       </c>
       <c r="L24" s="12"/>
       <c r="M24" s="3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -2216,12 +2292,16 @@
       <c r="D25" s="3"/>
       <c r="E25" s="4"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="4"/>
+      <c r="G25" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H25" s="5"/>
       <c r="I25" s="4"/>
       <c r="J25" s="5"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="12"/>
+      <c r="L25" s="12" t="s">
+        <v>380</v>
+      </c>
       <c r="M25" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -2241,7 +2321,7 @@
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="28" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="3" t="s">
         <v>221</v>
@@ -2249,18 +2329,18 @@
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H28" s="5"/>
       <c r="I28" s="4"/>
       <c r="J28" s="5"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="3" t="s">
-        <v>370</v>
-      </c>
+      <c r="L28" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="M28" s="3"/>
     </row>
     <row r="30" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -2288,7 +2368,9 @@
       <c r="D31" s="3"/>
       <c r="E31" s="4"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="4"/>
+      <c r="G31" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H31" s="5"/>
       <c r="I31" s="4"/>
       <c r="J31" s="5"/>
@@ -2305,7 +2387,9 @@
       <c r="D32" s="3"/>
       <c r="E32" s="4"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="4"/>
+      <c r="G32" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H32" s="5"/>
       <c r="I32" s="4"/>
       <c r="J32" s="5"/>
@@ -2322,7 +2406,9 @@
       <c r="D33" s="3"/>
       <c r="E33" s="4"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="4"/>
+      <c r="G33" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H33" s="5"/>
       <c r="I33" s="4"/>
       <c r="J33" s="5"/>
@@ -2339,7 +2425,9 @@
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
       <c r="F34" s="11"/>
-      <c r="G34" s="4"/>
+      <c r="G34" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H34" s="5"/>
       <c r="I34" s="4"/>
       <c r="J34" s="5"/>
@@ -2364,7 +2452,7 @@
       <c r="J35" s="5"/>
       <c r="K35" s="4"/>
       <c r="L35" s="12" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="M35" s="3"/>
     </row>
@@ -2385,7 +2473,7 @@
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
     </row>
-    <row r="38" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>227</v>
@@ -2393,60 +2481,92 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G38" s="4"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H38" s="5"/>
       <c r="I38" s="4"/>
       <c r="J38" s="5"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="3" t="s">
-        <v>342</v>
-      </c>
+      <c r="L38" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="M38" s="3"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="C39" s="3" t="s">
+        <v>385</v>
+      </c>
       <c r="D39" s="3"/>
       <c r="E39" s="4"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="4"/>
       <c r="J39" s="5"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="12"/>
+      <c r="L39" s="12" t="s">
+        <v>389</v>
+      </c>
       <c r="M39" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-    </row>
-    <row r="42" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="M40" s="3"/>
+    </row>
+    <row r="41" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+      <c r="G41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="M41" s="3"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="3"/>
-      <c r="B42" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3" t="s">
+        <v>393</v>
+      </c>
       <c r="D42" s="3"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="5"/>
+      <c r="F42" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G42" s="4"/>
       <c r="H42" s="5"/>
       <c r="I42" s="4"/>
@@ -2454,15 +2574,15 @@
       <c r="K42" s="4"/>
       <c r="L42" s="12"/>
       <c r="M42" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A43" s="3"/>
-      <c r="B43" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3" t="s">
+        <v>394</v>
+      </c>
       <c r="D43" s="3"/>
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
@@ -2470,18 +2590,20 @@
       <c r="H43" s="5"/>
       <c r="I43" s="4"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="4"/>
+      <c r="K43" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L43" s="12"/>
       <c r="M43" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
-      <c r="B44" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3" t="s">
+        <v>396</v>
+      </c>
       <c r="D44" s="3"/>
       <c r="E44" s="4"/>
       <c r="F44" s="5"/>
@@ -2489,76 +2611,61 @@
       <c r="H44" s="5"/>
       <c r="I44" s="4"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="4"/>
+      <c r="K44" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L44" s="12"/>
       <c r="M44" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="3"/>
-      <c r="B45" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="C45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>395</v>
+      </c>
       <c r="D45" s="3"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="5"/>
+      <c r="F45" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G45" s="4"/>
       <c r="H45" s="5"/>
       <c r="I45" s="4"/>
       <c r="J45" s="5"/>
       <c r="K45" s="4"/>
       <c r="L45" s="12"/>
-      <c r="M45" s="3"/>
-    </row>
-    <row r="46" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="3"/>
-    </row>
-    <row r="48" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M45" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+    </row>
+    <row r="48" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="3"/>
       <c r="B48" s="3" t="s">
-        <v>344</v>
+        <v>229</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="4"/>
-      <c r="F48" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F48" s="5"/>
       <c r="G48" s="4"/>
       <c r="H48" s="5"/>
       <c r="I48" s="4"/>
@@ -2566,13 +2673,13 @@
       <c r="K48" s="4"/>
       <c r="L48" s="12"/>
       <c r="M48" s="3" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A49" s="3"/>
       <c r="B49" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -2584,12 +2691,14 @@
       <c r="J49" s="5"/>
       <c r="K49" s="4"/>
       <c r="L49" s="12"/>
-      <c r="M49" s="3"/>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M49" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -2601,12 +2710,14 @@
       <c r="J50" s="5"/>
       <c r="K50" s="4"/>
       <c r="L50" s="12"/>
-      <c r="M50" s="3"/>
-    </row>
-    <row r="51" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M50" s="3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -2620,17 +2731,15 @@
       <c r="L51" s="12"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A52" s="3"/>
       <c r="B52" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
       <c r="E52" s="4"/>
-      <c r="F52" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F52" s="5"/>
       <c r="G52" s="4"/>
       <c r="H52" s="5"/>
       <c r="I52" s="4"/>
@@ -2638,20 +2747,18 @@
       <c r="K52" s="4"/>
       <c r="L52" s="12"/>
       <c r="M52" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="3"/>
       <c r="B53" s="3" t="s">
-        <v>238</v>
+        <v>343</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F53" s="5"/>
       <c r="G53" s="4"/>
       <c r="H53" s="5"/>
       <c r="I53" s="4"/>
@@ -2660,44 +2767,65 @@
       <c r="L53" s="12"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
       <c r="B54" s="3" t="s">
-        <v>239</v>
+        <v>344</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="4"/>
-      <c r="F54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G54" s="4"/>
       <c r="H54" s="5"/>
       <c r="I54" s="4"/>
       <c r="J54" s="5"/>
       <c r="K54" s="4"/>
       <c r="L54" s="12"/>
-      <c r="M54" s="3"/>
-    </row>
-    <row r="56" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="I56" s="7"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="7"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
+      <c r="M54" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="12"/>
+      <c r="M55" s="3"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="12"/>
+      <c r="M56" s="3"/>
     </row>
     <row r="57" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="3"/>
       <c r="B57" s="3" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -2711,10 +2839,10 @@
       <c r="L57" s="12"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="3"/>
       <c r="B58" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -2729,13 +2857,13 @@
       <c r="K58" s="4"/>
       <c r="L58" s="12"/>
       <c r="M58" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" s="3"/>
       <c r="B59" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -2749,85 +2877,48 @@
       <c r="J59" s="5"/>
       <c r="K59" s="4"/>
       <c r="L59" s="12"/>
-      <c r="M59" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="M59" s="3"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" s="3"/>
       <c r="B60" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
       <c r="E60" s="4"/>
       <c r="F60" s="5"/>
-      <c r="G60" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="G60" s="4"/>
       <c r="H60" s="5"/>
       <c r="I60" s="4"/>
       <c r="J60" s="5"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="M60" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="4"/>
-      <c r="L61" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="M61" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="5"/>
-      <c r="K62" s="4"/>
-      <c r="L62" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>352</v>
-      </c>
+      <c r="L60" s="12"/>
+      <c r="M60" s="3"/>
+    </row>
+    <row r="62" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A62" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+      <c r="I62" s="7"/>
+      <c r="J62" s="7"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
     </row>
     <row r="63" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3" t="s">
-        <v>247</v>
-      </c>
+      <c r="B63" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" s="3"/>
       <c r="D63" s="3"/>
       <c r="E63" s="4"/>
       <c r="F63" s="5"/>
@@ -2839,283 +2930,345 @@
       <c r="J63" s="5"/>
       <c r="K63" s="4"/>
       <c r="L63" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="M63" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+        <v>392</v>
+      </c>
+      <c r="M63" s="3"/>
+    </row>
+    <row r="64" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A64" s="3"/>
       <c r="B64" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
       <c r="E64" s="4"/>
-      <c r="F64" s="5"/>
+      <c r="F64" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G64" s="4"/>
       <c r="H64" s="5"/>
       <c r="I64" s="4"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="4"/>
+      <c r="K64" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L64" s="12"/>
-      <c r="M64" s="3"/>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M64" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-      <c r="C65" s="3" t="s">
-        <v>249</v>
-      </c>
+      <c r="B65" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="3"/>
       <c r="E65" s="4"/>
-      <c r="F65" s="5"/>
+      <c r="F65" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G65" s="4"/>
       <c r="H65" s="5"/>
       <c r="I65" s="4"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="4"/>
+      <c r="K65" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L65" s="12"/>
-      <c r="M65" s="3"/>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M65" s="3" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3" t="s">
-        <v>250</v>
-      </c>
+      <c r="B66" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C66" s="3"/>
       <c r="D66" s="3"/>
       <c r="E66" s="4"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="4"/>
+      <c r="G66" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H66" s="5"/>
       <c r="I66" s="4"/>
       <c r="J66" s="5"/>
       <c r="K66" s="4"/>
-      <c r="L66" s="12"/>
-      <c r="M66" s="3"/>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="7"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="7"/>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
-    </row>
-    <row r="69" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="L66" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M66" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="D67" s="3"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H67" s="5"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M67" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H68" s="5"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M68" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="3"/>
-      <c r="B69" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="C69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3" t="s">
+        <v>247</v>
+      </c>
       <c r="D69" s="3"/>
       <c r="E69" s="4"/>
-      <c r="F69" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G69" s="4"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H69" s="5"/>
       <c r="I69" s="4"/>
       <c r="J69" s="5"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="12"/>
+      <c r="L69" s="12" t="s">
+        <v>176</v>
+      </c>
       <c r="M69" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="70" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3" t="s">
-        <v>252</v>
-      </c>
+      <c r="B70" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C70" s="3"/>
       <c r="D70" s="3"/>
       <c r="E70" s="4"/>
-      <c r="F70" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F70" s="5"/>
       <c r="G70" s="4"/>
       <c r="H70" s="5"/>
       <c r="I70" s="4"/>
       <c r="J70" s="5"/>
       <c r="K70" s="4"/>
       <c r="L70" s="12"/>
-      <c r="M70" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="M70" s="3"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="C71" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D71" s="3"/>
       <c r="E71" s="4"/>
-      <c r="F71" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F71" s="5"/>
       <c r="G71" s="4"/>
       <c r="H71" s="5"/>
       <c r="I71" s="4"/>
       <c r="J71" s="5"/>
       <c r="K71" s="4"/>
       <c r="L71" s="12"/>
-      <c r="M71" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="M71" s="3"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3" t="s">
-        <v>254</v>
-      </c>
+      <c r="C72" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D72" s="3"/>
       <c r="E72" s="4"/>
-      <c r="F72" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F72" s="5"/>
       <c r="G72" s="4"/>
       <c r="H72" s="5"/>
       <c r="I72" s="4"/>
       <c r="J72" s="5"/>
       <c r="K72" s="4"/>
       <c r="L72" s="12"/>
-      <c r="M72" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G73" s="4"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="5"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="64" x14ac:dyDescent="0.2">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G74" s="4"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="4"/>
-      <c r="J74" s="5"/>
-      <c r="K74" s="4"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="3" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="B76" s="6"/>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
-      <c r="I76" s="7"/>
-      <c r="J76" s="7"/>
-      <c r="K76" s="7"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-    </row>
-    <row r="77" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M72" s="3"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A74" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="I74" s="7"/>
+      <c r="J74" s="7"/>
+      <c r="K74" s="7"/>
+      <c r="L74" s="6"/>
+      <c r="M74" s="6"/>
+    </row>
+    <row r="75" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G75" s="4"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="12"/>
+      <c r="M75" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D76" s="3"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G76" s="4"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="5"/>
+      <c r="K76" s="4"/>
+      <c r="L76" s="12"/>
+      <c r="M76" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A77" s="3"/>
-      <c r="B77" s="3" t="s">
-        <v>361</v>
-      </c>
+      <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
+      <c r="D77" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="E77" s="4"/>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G77" s="4"/>
       <c r="H77" s="5"/>
       <c r="I77" s="4"/>
       <c r="J77" s="5"/>
       <c r="K77" s="4"/>
       <c r="L77" s="12"/>
-      <c r="M77" s="3"/>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A79" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="B79" s="6"/>
-      <c r="C79" s="6"/>
-      <c r="D79" s="6"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-    </row>
-    <row r="80" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M77" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="E78" s="4"/>
+      <c r="F78" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G78" s="4"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="4"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="4"/>
+      <c r="L78" s="12"/>
+      <c r="M78" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G79" s="4"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="4"/>
+      <c r="J79" s="5"/>
+      <c r="K79" s="4"/>
+      <c r="L79" s="12"/>
+      <c r="M79" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="3"/>
-      <c r="B80" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="C80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3" t="s">
+        <v>256</v>
+      </c>
       <c r="D80" s="3"/>
       <c r="E80" s="4"/>
-      <c r="F80" s="5"/>
+      <c r="F80" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="G80" s="4"/>
       <c r="H80" s="5"/>
       <c r="I80" s="4"/>
       <c r="J80" s="5"/>
-      <c r="K80" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L80" s="12" t="s">
-        <v>354</v>
-      </c>
+      <c r="K80" s="4"/>
+      <c r="L80" s="12"/>
       <c r="M80" s="3" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B82" s="6"/>
       <c r="C82" s="6"/>
@@ -3130,101 +3283,70 @@
       <c r="L82" s="6"/>
       <c r="M82" s="6"/>
     </row>
-    <row r="83" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A83" s="3"/>
       <c r="B83" s="3" t="s">
-        <v>261</v>
+        <v>359</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
       <c r="E83" s="4"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="F83" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G83" s="4"/>
       <c r="H83" s="5"/>
       <c r="I83" s="4"/>
       <c r="J83" s="5"/>
       <c r="K83" s="4"/>
-      <c r="L83" s="12" t="s">
-        <v>180</v>
-      </c>
+      <c r="L83" s="12"/>
       <c r="M83" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-      <c r="B84" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="5"/>
-      <c r="G84" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="4"/>
-      <c r="J84" s="5"/>
-      <c r="K84" s="4"/>
-      <c r="L84" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="M84" s="3" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="5"/>
-      <c r="G85" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H85" s="5"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="5"/>
-      <c r="K85" s="4"/>
-      <c r="L85" s="12" t="s">
-        <v>180</v>
-      </c>
-      <c r="M85" s="3" t="s">
-        <v>355</v>
-      </c>
+      <c r="A85" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
     </row>
     <row r="86" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3"/>
       <c r="B86" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
       <c r="E86" s="4"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="G86" s="4"/>
       <c r="H86" s="5"/>
       <c r="I86" s="4"/>
       <c r="J86" s="5"/>
-      <c r="K86" s="4"/>
+      <c r="K86" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L86" s="12" t="s">
-        <v>180</v>
+        <v>354</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="6"/>
@@ -3242,7 +3364,7 @@
     <row r="89" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="3"/>
       <c r="B89" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -3265,7 +3387,7 @@
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" s="3"/>
       <c r="B90" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -3285,10 +3407,10 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" s="3"/>
       <c r="B91" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -3308,152 +3430,155 @@
         <v>355</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="B93" s="6"/>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="7"/>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7"/>
-      <c r="H93" s="7"/>
-      <c r="I93" s="7"/>
-      <c r="J93" s="7"/>
-      <c r="K93" s="7"/>
-      <c r="L93" s="6"/>
-      <c r="M93" s="6"/>
-    </row>
-    <row r="94" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A94" s="3"/>
-      <c r="B94" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="4"/>
-      <c r="F94" s="5"/>
-      <c r="G94" s="4"/>
-      <c r="H94" s="5"/>
-      <c r="I94" s="4"/>
-      <c r="J94" s="5"/>
-      <c r="K94" s="4"/>
-      <c r="L94" s="12"/>
-      <c r="M94" s="3"/>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A92" s="3"/>
+      <c r="B92" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="4"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H92" s="5"/>
+      <c r="I92" s="4"/>
+      <c r="J92" s="5"/>
+      <c r="K92" s="4"/>
+      <c r="L92" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A94" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="B94" s="6"/>
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+    </row>
+    <row r="95" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="3"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3" t="s">
-        <v>270</v>
-      </c>
+      <c r="B95" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C95" s="3"/>
       <c r="D95" s="3"/>
       <c r="E95" s="4"/>
       <c r="F95" s="5"/>
-      <c r="G95" s="4"/>
+      <c r="G95" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H95" s="5"/>
       <c r="I95" s="4"/>
       <c r="J95" s="5"/>
       <c r="K95" s="4"/>
-      <c r="L95" s="12"/>
-      <c r="M95" s="3"/>
+      <c r="L95" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="M95" s="3" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" s="3"/>
-      <c r="B96" s="3"/>
+      <c r="B96" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="C96" s="3"/>
-      <c r="D96" s="3" t="s">
-        <v>271</v>
-      </c>
+      <c r="D96" s="3"/>
       <c r="E96" s="4"/>
       <c r="F96" s="5"/>
-      <c r="G96" s="4"/>
+      <c r="G96" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H96" s="5"/>
       <c r="I96" s="4"/>
       <c r="J96" s="5"/>
       <c r="K96" s="4"/>
-      <c r="L96" s="12"/>
-      <c r="M96" s="3"/>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="L96" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="M96" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="3"/>
-      <c r="B97" s="3"/>
+      <c r="B97" s="3" t="s">
+        <v>264</v>
+      </c>
       <c r="C97" s="3"/>
-      <c r="D97" s="3" t="s">
-        <v>272</v>
-      </c>
+      <c r="D97" s="3"/>
       <c r="E97" s="4"/>
       <c r="F97" s="5"/>
-      <c r="G97" s="4"/>
+      <c r="G97" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H97" s="5"/>
       <c r="I97" s="4"/>
       <c r="J97" s="5"/>
       <c r="K97" s="4"/>
-      <c r="L97" s="12"/>
-      <c r="M97" s="3"/>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A98" s="3"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="E98" s="4"/>
-      <c r="F98" s="5"/>
-      <c r="G98" s="4"/>
-      <c r="H98" s="5"/>
-      <c r="I98" s="4"/>
-      <c r="J98" s="5"/>
-      <c r="K98" s="4"/>
-      <c r="L98" s="12"/>
-      <c r="M98" s="3"/>
-    </row>
-    <row r="99" spans="1:13" ht="48" x14ac:dyDescent="0.2">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="4"/>
-      <c r="F99" s="5"/>
-      <c r="G99" s="4"/>
-      <c r="H99" s="5"/>
-      <c r="I99" s="4"/>
-      <c r="J99" s="5"/>
-      <c r="K99" s="4"/>
-      <c r="L99" s="12"/>
-      <c r="M99" s="3"/>
-    </row>
-    <row r="100" spans="1:13" ht="64" x14ac:dyDescent="0.2">
+      <c r="L97" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="M97" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A99" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="7"/>
+      <c r="I99" s="7"/>
+      <c r="J99" s="7"/>
+      <c r="K99" s="7"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+    </row>
+    <row r="100" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="3"/>
       <c r="B100" s="3" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="4"/>
-      <c r="F100" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F100" s="5"/>
       <c r="G100" s="4"/>
       <c r="H100" s="5"/>
       <c r="I100" s="4"/>
       <c r="J100" s="5"/>
       <c r="K100" s="4"/>
       <c r="L100" s="12"/>
-      <c r="M100" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="101" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M100" s="3"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" s="3"/>
-      <c r="B101" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="3" t="s">
+        <v>270</v>
+      </c>
       <c r="D101" s="3"/>
       <c r="E101" s="4"/>
       <c r="F101" s="5"/>
@@ -3465,96 +3590,80 @@
       <c r="L101" s="12"/>
       <c r="M101" s="3"/>
     </row>
-    <row r="102" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="3"/>
-      <c r="B102" s="3" t="s">
-        <v>277</v>
-      </c>
+      <c r="B102" s="3"/>
       <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
+      <c r="D102" s="3" t="s">
+        <v>271</v>
+      </c>
       <c r="E102" s="4"/>
-      <c r="F102" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F102" s="5"/>
       <c r="G102" s="4"/>
       <c r="H102" s="5"/>
       <c r="I102" s="4"/>
       <c r="J102" s="5"/>
       <c r="K102" s="4"/>
       <c r="L102" s="12"/>
-      <c r="M102" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="103" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M102" s="3"/>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" s="3"/>
-      <c r="B103" s="3" t="s">
-        <v>278</v>
-      </c>
+      <c r="B103" s="3"/>
       <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>272</v>
+      </c>
       <c r="E103" s="4"/>
-      <c r="F103" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F103" s="5"/>
       <c r="G103" s="4"/>
       <c r="H103" s="5"/>
       <c r="I103" s="4"/>
       <c r="J103" s="5"/>
       <c r="K103" s="4"/>
       <c r="L103" s="12"/>
-      <c r="M103" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="104" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M103" s="3"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" s="3"/>
-      <c r="B104" s="3" t="s">
-        <v>279</v>
-      </c>
+      <c r="B104" s="3"/>
       <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
+      <c r="D104" s="3" t="s">
+        <v>273</v>
+      </c>
       <c r="E104" s="4"/>
-      <c r="F104" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F104" s="5"/>
       <c r="G104" s="4"/>
       <c r="H104" s="5"/>
       <c r="I104" s="4"/>
       <c r="J104" s="5"/>
       <c r="K104" s="4"/>
       <c r="L104" s="12"/>
-      <c r="M104" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="105" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M104" s="3"/>
+    </row>
+    <row r="105" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="3"/>
       <c r="B105" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="4"/>
-      <c r="F105" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F105" s="5"/>
       <c r="G105" s="4"/>
       <c r="H105" s="5"/>
       <c r="I105" s="4"/>
       <c r="J105" s="5"/>
       <c r="K105" s="4"/>
       <c r="L105" s="12"/>
-      <c r="M105" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="106" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M105" s="3"/>
+    </row>
+    <row r="106" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A106" s="3"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3" t="s">
-        <v>281</v>
-      </c>
+      <c r="B106" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="4"/>
       <c r="F106" s="5" t="s">
@@ -3567,13 +3676,13 @@
       <c r="K106" s="4"/>
       <c r="L106" s="12"/>
       <c r="M106" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="3"/>
       <c r="B107" s="3" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -3583,21 +3692,25 @@
       <c r="H107" s="5"/>
       <c r="I107" s="4"/>
       <c r="J107" s="5"/>
-      <c r="K107" s="4"/>
-      <c r="L107" s="12"/>
-      <c r="M107" s="3"/>
-    </row>
-    <row r="108" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="K107" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L107" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="M107" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" ht="288" x14ac:dyDescent="0.2">
       <c r="A108" s="3"/>
       <c r="B108" s="3" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
       <c r="E108" s="4"/>
-      <c r="F108" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F108" s="5"/>
       <c r="G108" s="4"/>
       <c r="H108" s="5"/>
       <c r="I108" s="4"/>
@@ -3605,37 +3718,56 @@
       <c r="K108" s="4"/>
       <c r="L108" s="12"/>
       <c r="M108" s="3" t="s">
-        <v>366</v>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A109" s="3"/>
+      <c r="B109" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
+      <c r="E109" s="4"/>
+      <c r="F109" s="5"/>
+      <c r="G109" s="4"/>
+      <c r="H109" s="5"/>
+      <c r="I109" s="4"/>
+      <c r="J109" s="5"/>
+      <c r="K109" s="4"/>
+      <c r="L109" s="12"/>
+      <c r="M109" s="3" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="B110" s="6"/>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="7"/>
-      <c r="F110" s="7"/>
-      <c r="G110" s="7"/>
-      <c r="H110" s="7"/>
-      <c r="I110" s="7"/>
-      <c r="J110" s="7"/>
-      <c r="K110" s="7"/>
-      <c r="L110" s="6"/>
-      <c r="M110" s="6"/>
-    </row>
-    <row r="111" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
+      <c r="E110" s="4"/>
+      <c r="F110" s="5"/>
+      <c r="G110" s="4"/>
+      <c r="H110" s="5"/>
+      <c r="I110" s="4"/>
+      <c r="J110" s="5"/>
+      <c r="K110" s="4"/>
+      <c r="L110" s="12"/>
+      <c r="M110" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" s="3"/>
       <c r="B111" s="3" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
       <c r="E111" s="4"/>
-      <c r="F111" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F111" s="5"/>
       <c r="G111" s="4"/>
       <c r="H111" s="5"/>
       <c r="I111" s="4"/>
@@ -3643,20 +3775,18 @@
       <c r="K111" s="4"/>
       <c r="L111" s="12"/>
       <c r="M111" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="112" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="4"/>
-      <c r="F112" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F112" s="5"/>
       <c r="G112" s="4"/>
       <c r="H112" s="5"/>
       <c r="I112" s="4"/>
@@ -3664,36 +3794,32 @@
       <c r="K112" s="4"/>
       <c r="L112" s="12"/>
       <c r="M112" s="3" t="s">
-        <v>357</v>
+        <v>403</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A113" s="3"/>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3" t="s">
-        <v>272</v>
-      </c>
+      <c r="B113" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C113" s="3"/>
       <c r="D113" s="3"/>
       <c r="E113" s="4"/>
-      <c r="F113" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F113" s="5"/>
       <c r="G113" s="4"/>
       <c r="H113" s="5"/>
       <c r="I113" s="4"/>
       <c r="J113" s="5"/>
       <c r="K113" s="4"/>
       <c r="L113" s="12"/>
-      <c r="M113" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="114" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M113" s="3"/>
+    </row>
+    <row r="114" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A114" s="3"/>
-      <c r="B114" s="3"/>
-      <c r="C114" s="3" t="s">
-        <v>273</v>
-      </c>
+      <c r="B114" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="C114" s="3"/>
       <c r="D114" s="3"/>
       <c r="E114" s="4"/>
       <c r="F114" s="5" t="s">
@@ -3706,55 +3832,30 @@
       <c r="K114" s="4"/>
       <c r="L114" s="12"/>
       <c r="M114" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="4"/>
-      <c r="F115" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G115" s="4"/>
-      <c r="H115" s="5"/>
-      <c r="I115" s="4"/>
-      <c r="J115" s="5"/>
-      <c r="K115" s="4"/>
-      <c r="L115" s="12"/>
-      <c r="M115" s="3" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="4"/>
-      <c r="F116" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G116" s="4"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="4"/>
-      <c r="J116" s="5"/>
-      <c r="K116" s="4"/>
-      <c r="L116" s="12"/>
-      <c r="M116" s="3" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="117" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="B116" s="6"/>
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7"/>
+      <c r="H116" s="7"/>
+      <c r="I116" s="7"/>
+      <c r="J116" s="7"/>
+      <c r="K116" s="7"/>
+      <c r="L116" s="6"/>
+      <c r="M116" s="6"/>
+    </row>
+    <row r="117" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A117" s="3"/>
       <c r="B117" s="3" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -3764,16 +3865,20 @@
       <c r="H117" s="5"/>
       <c r="I117" s="4"/>
       <c r="J117" s="5"/>
-      <c r="K117" s="4"/>
+      <c r="K117" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L117" s="12"/>
-      <c r="M117" s="3"/>
-    </row>
-    <row r="118" spans="1:13" ht="80" x14ac:dyDescent="0.2">
+      <c r="M117" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="3"/>
-      <c r="B118" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="C118" s="3"/>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3" t="s">
+        <v>271</v>
+      </c>
       <c r="D118" s="3"/>
       <c r="E118" s="4"/>
       <c r="F118" s="5"/>
@@ -3781,31 +3886,60 @@
       <c r="H118" s="5"/>
       <c r="I118" s="4"/>
       <c r="J118" s="5"/>
-      <c r="K118" s="4"/>
+      <c r="K118" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L118" s="12"/>
-      <c r="M118" s="3"/>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A120" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="7"/>
-      <c r="F120" s="7"/>
-      <c r="G120" s="7"/>
-      <c r="H120" s="7"/>
-      <c r="I120" s="7"/>
-      <c r="J120" s="7"/>
-      <c r="K120" s="7"/>
-      <c r="L120" s="6"/>
-      <c r="M120" s="6"/>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M118" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A119" s="3"/>
+      <c r="B119" s="3"/>
+      <c r="C119" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D119" s="3"/>
+      <c r="E119" s="4"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="4"/>
+      <c r="H119" s="5"/>
+      <c r="I119" s="4"/>
+      <c r="J119" s="5"/>
+      <c r="K119" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L119" s="12"/>
+      <c r="M119" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" ht="48" x14ac:dyDescent="0.2">
+      <c r="A120" s="3"/>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="4"/>
+      <c r="F120" s="5"/>
+      <c r="G120" s="4"/>
+      <c r="H120" s="5"/>
+      <c r="I120" s="4"/>
+      <c r="J120" s="5"/>
+      <c r="K120" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L120" s="12"/>
+      <c r="M120" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="3"/>
       <c r="B121" s="3" t="s">
-        <v>363</v>
+        <v>285</v>
       </c>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -3815,16 +3949,20 @@
       <c r="H121" s="5"/>
       <c r="I121" s="4"/>
       <c r="J121" s="5"/>
-      <c r="K121" s="4"/>
+      <c r="K121" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L121" s="12"/>
-      <c r="M121" s="3"/>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M121" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" ht="48" x14ac:dyDescent="0.2">
       <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3" t="s">
-        <v>290</v>
-      </c>
+      <c r="B122" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C122" s="3"/>
       <c r="D122" s="3"/>
       <c r="E122" s="4"/>
       <c r="F122" s="5"/>
@@ -3832,16 +3970,20 @@
       <c r="H122" s="5"/>
       <c r="I122" s="4"/>
       <c r="J122" s="5"/>
-      <c r="K122" s="4"/>
+      <c r="K122" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="L122" s="12"/>
-      <c r="M122" s="3"/>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M122" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3" t="s">
-        <v>199</v>
-      </c>
+      <c r="B123" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C123" s="3"/>
       <c r="D123" s="3"/>
       <c r="E123" s="4"/>
       <c r="F123" s="5"/>
@@ -3853,12 +3995,12 @@
       <c r="L123" s="12"/>
       <c r="M123" s="3"/>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3" t="s">
-        <v>291</v>
-      </c>
+      <c r="B124" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C124" s="3"/>
       <c r="D124" s="3"/>
       <c r="E124" s="4"/>
       <c r="F124" s="5"/>
@@ -3870,152 +4012,237 @@
       <c r="L124" s="12"/>
       <c r="M124" s="3"/>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="D125" s="3"/>
-      <c r="E125" s="4"/>
-      <c r="F125" s="5"/>
-      <c r="G125" s="4"/>
-      <c r="H125" s="5"/>
-      <c r="I125" s="4"/>
-      <c r="J125" s="5"/>
-      <c r="K125" s="4"/>
-      <c r="L125" s="12"/>
-      <c r="M125" s="3"/>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A126" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
+      <c r="G126" s="7"/>
+      <c r="H126" s="7"/>
+      <c r="I126" s="7"/>
+      <c r="J126" s="7"/>
+      <c r="K126" s="7"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A127" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="B127" s="6"/>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="7"/>
-      <c r="F127" s="7"/>
-      <c r="G127" s="7"/>
-      <c r="H127" s="7"/>
-      <c r="I127" s="7"/>
-      <c r="J127" s="7"/>
-      <c r="K127" s="7"/>
-      <c r="L127" s="6"/>
-      <c r="M127" s="6"/>
-    </row>
-    <row r="128" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
+      <c r="E127" s="4"/>
+      <c r="F127" s="5"/>
+      <c r="G127" s="4"/>
+      <c r="H127" s="5"/>
+      <c r="I127" s="4"/>
+      <c r="J127" s="5"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="12"/>
+      <c r="M127" s="3"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" s="3"/>
-      <c r="B128" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="C128" s="3"/>
+      <c r="B128" s="3"/>
+      <c r="C128" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="D128" s="3"/>
       <c r="E128" s="4"/>
-      <c r="F128" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F128" s="5"/>
       <c r="G128" s="4"/>
       <c r="H128" s="5"/>
       <c r="I128" s="4"/>
       <c r="J128" s="5"/>
       <c r="K128" s="4"/>
       <c r="L128" s="12"/>
-      <c r="M128" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="129" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M128" s="3"/>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" s="3"/>
-      <c r="B129" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C129" s="3"/>
+      <c r="B129" s="3"/>
+      <c r="C129" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="D129" s="3"/>
       <c r="E129" s="4"/>
-      <c r="F129" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F129" s="5"/>
       <c r="G129" s="4"/>
       <c r="H129" s="5"/>
       <c r="I129" s="4"/>
       <c r="J129" s="5"/>
       <c r="K129" s="4"/>
       <c r="L129" s="12"/>
-      <c r="M129" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="130" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="M129" s="3"/>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" s="3"/>
-      <c r="B130" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="C130" s="3"/>
+      <c r="B130" s="3"/>
+      <c r="C130" s="3" t="s">
+        <v>291</v>
+      </c>
       <c r="D130" s="3"/>
       <c r="E130" s="4"/>
-      <c r="F130" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="F130" s="5"/>
       <c r="G130" s="4"/>
       <c r="H130" s="5"/>
       <c r="I130" s="4"/>
       <c r="J130" s="5"/>
       <c r="K130" s="4"/>
       <c r="L130" s="12"/>
-      <c r="M130" s="3" t="s">
+      <c r="M130" s="3"/>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D131" s="3"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="5"/>
+      <c r="G131" s="4"/>
+      <c r="H131" s="5"/>
+      <c r="I131" s="4"/>
+      <c r="J131" s="5"/>
+      <c r="K131" s="4"/>
+      <c r="L131" s="12"/>
+      <c r="M131" s="3"/>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A133" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="B133" s="6"/>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7"/>
+      <c r="G133" s="7"/>
+      <c r="H133" s="7"/>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="6"/>
+      <c r="M133" s="6"/>
+    </row>
+    <row r="134" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A134" s="3"/>
+      <c r="B134" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
+      <c r="E134" s="4"/>
+      <c r="F134" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G134" s="4"/>
+      <c r="H134" s="5"/>
+      <c r="I134" s="4"/>
+      <c r="J134" s="5"/>
+      <c r="K134" s="4"/>
+      <c r="L134" s="12"/>
+      <c r="M134" s="3" t="s">
         <v>342</v>
       </c>
     </row>
+    <row r="135" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A135" s="3"/>
+      <c r="B135" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
+      <c r="E135" s="4"/>
+      <c r="F135" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G135" s="4"/>
+      <c r="H135" s="5"/>
+      <c r="I135" s="4"/>
+      <c r="J135" s="5"/>
+      <c r="K135" s="4"/>
+      <c r="L135" s="12"/>
+      <c r="M135" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A136" s="3"/>
+      <c r="B136" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
+      <c r="E136" s="4"/>
+      <c r="F136" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G136" s="4"/>
+      <c r="H136" s="5"/>
+      <c r="I136" s="4"/>
+      <c r="J136" s="5"/>
+      <c r="K136" s="4"/>
+      <c r="L136" s="12"/>
+      <c r="M136" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F92 F109 F131:F1048576 F119:F126 F1:F87">
+  <conditionalFormatting sqref="F98 F115 F137:F1048576 F125:F132 F1:F40 F42:F93">
     <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K92 G92 G109 K109 K131:K1048576 G131:G1048576 G119:G126 K119:K126 G1:G87 K1:K87">
+  <conditionalFormatting sqref="K98 G98 G115 K115 K137:K1048576 G137:G1048576 G125:G132 K125:K132 G1:G93 K1:K93">
     <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F88:F91">
+  <conditionalFormatting sqref="F94:F97">
     <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",F88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",F94)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G88:G91 K88:K91">
+  <conditionalFormatting sqref="G94:G97 K94:K97">
     <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",G88)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",G94)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F93:F108">
+  <conditionalFormatting sqref="F99:F114">
     <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",F93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",F99)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G93:G108 K93:K108">
+  <conditionalFormatting sqref="G99:G114 K99:K114">
     <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",G93)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",G99)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F110:F118">
+  <conditionalFormatting sqref="F116:F124">
     <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",F110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",F116)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G110:G118 K110:K118">
+  <conditionalFormatting sqref="G116:G124 K116:K124">
     <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",G110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",G116)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F127:F130">
+  <conditionalFormatting sqref="F133:F136">
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",F127)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",F133)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G127:G130 K127:K130">
+  <conditionalFormatting sqref="G133:G136 K133:K136">
     <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",G127)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Y",G133)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4027,8 +4254,8 @@
   <dimension ref="A1:Q128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4:K128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4162,7 +4389,7 @@
       <c r="J6" s="5"/>
       <c r="K6" s="4"/>
       <c r="L6" s="12" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>297</v>
@@ -6617,6 +6844,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1"/>
   <conditionalFormatting sqref="F1:F1048576">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",F1)))</formula>

</xml_diff>

<commit_message>
Merged in external docs
</commit_message>
<xml_diff>
--- a/artifacts/project/HDInsight Dev Guide Status.xlsx
+++ b/artifacts/project/HDInsight Dev Guide Status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="22500" windowHeight="9945" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22500" windowHeight="9945" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Milestone 2" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Milestone 1'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="171027" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="435">
   <si>
     <t>Topic</t>
   </si>
@@ -1905,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M126" sqref="M126"/>
     </sheetView>
   </sheetViews>
@@ -4763,9 +4762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4856,7 +4855,9 @@
       <c r="G4" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
       <c r="K4" s="5"/>
@@ -4878,7 +4879,9 @@
       <c r="G5" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I5" s="5"/>
       <c r="J5" s="4"/>
       <c r="K5" s="5"/>
@@ -5045,7 +5048,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
@@ -5168,7 +5171,9 @@
       <c r="G18" s="5" t="s">
         <v>397</v>
       </c>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4"/>
       <c r="K18" s="5"/>
@@ -6100,7 +6105,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>62</v>
       </c>
@@ -6965,7 +6970,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>96</v>
       </c>
@@ -7063,7 +7068,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
         <v>99</v>
       </c>
@@ -7127,7 +7132,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>102</v>
       </c>
@@ -7310,7 +7315,7 @@
       </c>
       <c r="N118" s="3"/>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>305</v>
       </c>

</xml_diff>